<commit_message>
400 20 8 t
</commit_message>
<xml_diff>
--- a/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
+++ b/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\OneDrive - Universidad de Los Andes\2016-2\InfraComp\InfraCompCase2\InfraCompCase2\TABLAS PARA EL CASO 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseg\Desktop\WorkSpaces\WorkSpace Infracomp\Workspace Caso 2\TABLAS PARA EL CASO 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Esc 3" sheetId="1" r:id="rId1"/>
@@ -267,7 +267,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -699,7 +699,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1110,7 +1110,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1516,7 +1516,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1922,7 +1922,7 @@
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2337,7 +2337,7 @@
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2747,7 +2747,7 @@
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3157,7 +3157,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3614,7 +3614,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4061,7 +4061,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4136,34 +4136,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4495,7 +4495,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4952,7 +4952,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5399,7 +5399,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5474,34 +5474,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>3.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5833,7 +5833,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6290,7 +6290,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -13763,7 +13763,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -14065,7 +14065,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
@@ -14294,7 +14294,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -14519,7 +14519,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
@@ -14750,7 +14750,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
@@ -14997,7 +14997,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
@@ -15223,7 +15223,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
@@ -15448,7 +15448,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
@@ -15674,11 +15674,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -15823,34 +15823,34 @@
         <v>18</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
@@ -15858,34 +15858,34 @@
         <v>19</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="G7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="H7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="I7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="J7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="K7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
       <c r="L7" s="4">
-        <v>1</v>
+        <v>3.33</v>
       </c>
     </row>
   </sheetData>
@@ -15897,11 +15897,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -16172,7 +16172,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
push de tiempos sin seguridad
</commit_message>
<xml_diff>
--- a/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
+++ b/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Esc 3" sheetId="1" r:id="rId1"/>
@@ -1279,34 +1279,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6004,34 +6004,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>7.2889999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14746,8 +14746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14950,38 +14950,37 @@
         <v>19</v>
       </c>
       <c r="C8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="D8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="E8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="F8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="G8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="H8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="I8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="J8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="K8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="L8" s="4">
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
       <c r="M8" s="4">
-        <f>SUM(C8:L8)/10</f>
-        <v>5</v>
+        <v>7.2889999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -15444,7 +15443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
push nuevos tiempos nuevas tablas
</commit_message>
<xml_diff>
--- a/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
+++ b/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Esc 3" sheetId="1" r:id="rId1"/>
@@ -6387,34 +6387,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>3.8159999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14061,8 +14061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14251,34 +14251,34 @@
         <v>19</v>
       </c>
       <c r="C8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="D8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="E8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="F8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="G8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="H8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="I8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="J8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="K8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
       <c r="L8" s="4">
-        <v>3</v>
+        <v>3.8159999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -16167,8 +16167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
push tiempos y sin seguridad
</commit_message>
<xml_diff>
--- a/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
+++ b/TABLAS PARA EL CASO 3/Tablas de casos SIN SEGURIDAD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Esc 3" sheetId="1" r:id="rId1"/>
@@ -1685,34 +1685,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6451,34 +6451,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>5.5250000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14061,8 +14061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14992,8 +14992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -15179,34 +15179,34 @@
         <v>19</v>
       </c>
       <c r="C8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="D8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="E8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="F8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="G8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="H8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="I8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="J8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="K8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
       <c r="L8" s="4">
-        <v>6</v>
+        <v>5.5250000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>